<commit_message>
Atualização da documentação (Documentação, Planilha de Reunião, ATA de reunião, Slides de Apresentação)
</commit_message>
<xml_diff>
--- a/Documentação/Planilha Reuniões - SENSFIT.xlsx
+++ b/Documentação/Planilha Reuniões - SENSFIT.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27624"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93C65D58-AC75-47B4-ACE2-E6BF41EB7AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3600C7-9560-4DDE-A561-393EC6FDE9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>SENSFIT - Reuniões</t>
   </si>
@@ -84,7 +84,7 @@
     <t>On-line</t>
   </si>
   <si>
-    <t>Giovanna Beltrão</t>
+    <t xml:space="preserve">Giovana Zukauskas </t>
   </si>
   <si>
     <t>Luiz Felipe</t>
@@ -93,7 +93,7 @@
     <t>Edição/ajustes do protótipo, requisitos na ferramenta de gestão, configuração do git hub, criação da planilha de reuniões, criação das regras de condução do projeto, estabelecido a dinamica do projeto</t>
   </si>
   <si>
-    <t xml:space="preserve">Giovana Zukauskas </t>
+    <t xml:space="preserve">Giovanna Beltrão </t>
   </si>
   <si>
     <t>Busca por inspirações para realização do protótipo</t>
@@ -106,6 +106,110 @@
   </si>
   <si>
     <t>Yasmim Silva</t>
+  </si>
+  <si>
+    <t>Protótipo dashboard, inicio do site, alterações na documentação</t>
+  </si>
+  <si>
+    <t>15/04/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site institucional, protótipo dashboard, tabela gestão
+de riscos. </t>
+  </si>
+  <si>
+    <t>16/04/2024</t>
+  </si>
+  <si>
+    <t>Site institucional, dashboard, vida útil dos
+ aparelhos</t>
+  </si>
+  <si>
+    <t>17/04/2024</t>
+  </si>
+  <si>
+    <t>Isaías</t>
+  </si>
+  <si>
+    <t>Dashboard, Banco de dados, site institucional</t>
+  </si>
+  <si>
+    <t>18/04/2024</t>
+  </si>
+  <si>
+    <t>Site institucional, Dashboard,Banco de dados</t>
+  </si>
+  <si>
+    <t>19/04/2024</t>
+  </si>
+  <si>
+    <t>Feedback, arquitetura de TI, Banco de dados</t>
+  </si>
+  <si>
+    <t>21/04/2024</t>
+  </si>
+  <si>
+    <t>Isaías e Yasmim</t>
+  </si>
+  <si>
+    <t>Foi definido as tarefas da semana de cada integrante</t>
+  </si>
+  <si>
+    <t>22/04/2024</t>
+  </si>
+  <si>
+    <t>Foi definido prioridades do projeto para a semana</t>
+  </si>
+  <si>
+    <t>23/04/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devido a semana de provas, não houve progresso. </t>
+  </si>
+  <si>
+    <t>24/04/2024</t>
+  </si>
+  <si>
+    <t>Validações Concluídas e inicio da dashboard.</t>
+  </si>
+  <si>
+    <t>25/04/2024</t>
+  </si>
+  <si>
+    <t>Isaías - Justificado</t>
+  </si>
+  <si>
+    <t>Continuação da Dashboard,</t>
+  </si>
+  <si>
+    <t>26/04/2024</t>
+  </si>
+  <si>
+    <t>Continuação da Dashboard, ajustes nos textos do site</t>
+  </si>
+  <si>
+    <t>29/04/2024</t>
+  </si>
+  <si>
+    <t>Intensivão sobre o projeto, separação de partes</t>
+  </si>
+  <si>
+    <t>30/04/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giovanna, Isaias </t>
+  </si>
+  <si>
+    <t>Concluindo a dashboard, concluido slide</t>
+  </si>
+  <si>
+    <t>Treinado apresentação</t>
+  </si>
+  <si>
+    <t>Termino da documentação, sensores coletando dados e mandando para VM, treino da apresentação</t>
+  </si>
+  <si>
+    <t>Treino da apresentação</t>
   </si>
 </sst>
 </file>
@@ -170,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,11 +297,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,7 +362,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -226,6 +370,63 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,52 +768,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="H1" s="9" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -620,7 +822,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="29.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3">
@@ -690,7 +892,7 @@
     </row>
     <row r="6" spans="1:8" ht="29.25">
       <c r="A6" s="2">
-        <v>45539</v>
+        <v>45508</v>
       </c>
       <c r="B6" s="3">
         <v>0.79166666666666663</v>
@@ -712,42 +914,375 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.5">
-      <c r="A7" s="2">
+      <c r="A7" s="10">
         <v>45600</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="11">
         <v>0.69444444444444442</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="11">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="7"/>
+    <row r="8" spans="1:8" ht="29.25">
+      <c r="A8" s="18">
+        <v>45630</v>
+      </c>
+      <c r="B8" s="19">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.5">
+      <c r="A9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="21">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="29.25">
+      <c r="A10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="21">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C10" s="21">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="22.5" customHeight="1">
+      <c r="A11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="24">
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="C11" s="24">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="7"/>
+      <c r="A12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="21">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C12" s="21">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="7"/>
+      <c r="A13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="21">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C13" s="21">
+        <v>0.8125</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="24">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C14" s="24">
+        <v>0.875</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="19">
+        <v>0.6875</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="19">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C16" s="19">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0.8125</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="27">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C18" s="27">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="27">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.8125</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0.875</v>
+      </c>
+      <c r="C20" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="27">
+        <v>0.6875</v>
+      </c>
+      <c r="C21" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="23">
+        <v>45296</v>
+      </c>
+      <c r="B22" s="24">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C22" s="24">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29.25">
+      <c r="A23" s="18">
+        <v>45327</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="15">
+        <v>45356</v>
+      </c>
+      <c r="B24" s="21">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C24" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>